<commit_message>
🔧 chore(analisis): Actualizar archivo de análisis de homogeneidad de varianzas para reflejar cambios recientes en los datos.
</commit_message>
<xml_diff>
--- a/analisis/02_PASO2_LEVENE_HOMOGENEIDAD_VARIANZAS.xlsx
+++ b/analisis/02_PASO2_LEVENE_HOMOGENEIDAD_VARIANZAS.xlsx
@@ -7,8 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Levene_N2480" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Levene_N12" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Levene" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,8 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -29,13 +30,23 @@
     <font>
       <b val="1"/>
     </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="004472C4"/>
+        <bgColor rgb="004472C4"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -56,10 +67,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -433,415 +456,203 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="10" customWidth="1" min="1" max="1"/>
+    <col width="18" customWidth="1" min="2" max="2"/>
+    <col width="8" customWidth="1" min="3" max="3"/>
+    <col width="10" customWidth="1" min="4" max="4"/>
+    <col width="15" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="12" customWidth="1" min="8" max="8"/>
+    <col width="25" customWidth="1" min="9" max="9"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>nivel</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>metrica</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>n_ia</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>n_manual</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>var_ia</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>var_manual</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="2" t="inlineStr">
         <is>
           <t>F_statistic</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" s="2" t="inlineStr">
         <is>
           <t>p_value</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" s="2" t="inlineStr">
         <is>
           <t>es_igual</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>N=2,480</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>N=12</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
         <is>
           <t>instr_pct</t>
         </is>
       </c>
-      <c r="C2" t="n">
-        <v>880</v>
-      </c>
-      <c r="D2" t="n">
-        <v>1600</v>
-      </c>
-      <c r="E2" t="n">
-        <v>75.81825692625918</v>
-      </c>
-      <c r="F2" t="n">
-        <v>146.7718614133834</v>
-      </c>
-      <c r="G2" t="n">
-        <v>533.5283331422733</v>
-      </c>
-      <c r="H2" t="n">
-        <v>4.511579682431577e-107</v>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>✗ Varianzas DESIGUALES</t>
+      <c r="C2" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2" s="5" t="n">
+        <v>128.958333</v>
+      </c>
+      <c r="F2" s="5" t="n">
+        <v>156.370833</v>
+      </c>
+      <c r="G2" s="5" t="n">
+        <v>0.1006</v>
+      </c>
+      <c r="H2" s="5" t="n">
+        <v>0.7577</v>
+      </c>
+      <c r="I2" s="3" t="inlineStr">
+        <is>
+          <t>✓ Varianzas IGUALES</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>N=2,480</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>N=12</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
         <is>
           <t>branch_pct</t>
         </is>
       </c>
-      <c r="C3" t="n">
-        <v>880</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1600</v>
-      </c>
-      <c r="E3" t="n">
-        <v>45.53397940583307</v>
-      </c>
-      <c r="F3" t="n">
-        <v>153.5764540337711</v>
-      </c>
-      <c r="G3" t="n">
-        <v>167.3693488258101</v>
-      </c>
-      <c r="H3" t="n">
-        <v>4.292021191946926e-37</v>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>✗ Varianzas DESIGUALES</t>
+      <c r="C3" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="E3" s="5" t="n">
+        <v>159.159722</v>
+      </c>
+      <c r="F3" s="5" t="n">
+        <v>159.159722</v>
+      </c>
+      <c r="G3" s="5" t="n">
+        <v>0.1262</v>
+      </c>
+      <c r="H3" s="5" t="n">
+        <v>0.7298</v>
+      </c>
+      <c r="I3" s="3" t="inlineStr">
+        <is>
+          <t>✓ Varianzas IGUALES</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>N=2,480</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>N=12</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
         <is>
           <t>mutation_score</t>
         </is>
       </c>
-      <c r="C4" t="n">
-        <v>880</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1600</v>
-      </c>
-      <c r="E4" t="n">
-        <v>66.59469090857381</v>
-      </c>
-      <c r="F4" t="n">
-        <v>295.5828903064416</v>
-      </c>
-      <c r="G4" t="n">
-        <v>309.3370745605989</v>
-      </c>
-      <c r="H4" t="n">
-        <v>2.413048437614783e-65</v>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>✗ Varianzas DESIGUALES</t>
+      <c r="C4" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>313.128333</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <v>313.756667</v>
+      </c>
+      <c r="G4" s="5" t="n">
+        <v>0.393</v>
+      </c>
+      <c r="H4" s="5" t="n">
+        <v>0.5448</v>
+      </c>
+      <c r="I4" s="3" t="inlineStr">
+        <is>
+          <t>✓ Varianzas IGUALES</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>N=2,480</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>N=12</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
         <is>
           <t>time_seconds</t>
         </is>
       </c>
-      <c r="C5" t="n">
-        <v>880</v>
-      </c>
-      <c r="D5" t="n">
-        <v>1600</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.05371313128425897</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.03152233431480613</v>
-      </c>
-      <c r="G5" t="n">
-        <v>20.45811432561216</v>
-      </c>
-      <c r="H5" t="n">
-        <v>6.382191622667938e-06</v>
-      </c>
-      <c r="I5" t="inlineStr">
+      <c r="C5" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>0.007433</v>
+      </c>
+      <c r="F5" s="5" t="n">
+        <v>0.004736</v>
+      </c>
+      <c r="G5" s="5" t="n">
+        <v>6.3679</v>
+      </c>
+      <c r="H5" s="5" t="n">
+        <v>0.0302</v>
+      </c>
+      <c r="I5" s="3" t="inlineStr">
         <is>
           <t>✗ Varianzas DESIGUALES</t>
         </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>nivel</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>metrica</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>n_ia</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>n_manual</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>var_ia</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>var_manual</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>F_statistic</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>p_value</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>es_igual</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>ratio_var</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>N=12</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>instr_pct</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>6</v>
-      </c>
-      <c r="D2" t="n">
-        <v>6</v>
-      </c>
-      <c r="E2" t="n">
-        <v>129.098323375</v>
-      </c>
-      <c r="F2" t="n">
-        <v>156.3169366666667</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.1005534588048403</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.7576877767997356</v>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>✓ Varianzas IGUALES</t>
-        </is>
-      </c>
-      <c r="J2" t="n">
-        <v>1.210836303525051</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>N=12</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>branch_pct</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>6</v>
-      </c>
-      <c r="D3" t="n">
-        <v>6</v>
-      </c>
-      <c r="E3" t="n">
-        <v>90.09130859375</v>
-      </c>
-      <c r="F3" t="n">
-        <v>159.1666666666666</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.1261631285169443</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.7298213975322283</v>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>✓ Varianzas IGUALES</t>
-        </is>
-      </c>
-      <c r="J3" t="n">
-        <v>1.766726104339311</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>N=12</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>mutation_score</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>6</v>
-      </c>
-      <c r="D4" t="n">
-        <v>6</v>
-      </c>
-      <c r="E4" t="n">
-        <v>134.87492959375</v>
-      </c>
-      <c r="F4" t="n">
-        <v>313.75844</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.3930361867634057</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.5447541451208455</v>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>✓ Varianzas IGUALES</t>
-        </is>
-      </c>
-      <c r="J4" t="n">
-        <v>2.326291779688457</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>N=12</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>time_seconds</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>6</v>
-      </c>
-      <c r="D5" t="n">
-        <v>6</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.03729544366901042</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.004736459427878402</v>
-      </c>
-      <c r="G5" t="n">
-        <v>6.367874425075419</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.03020741164808924</v>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>✗ Varianzas DESIGUALES</t>
-        </is>
-      </c>
-      <c r="J5" t="n">
-        <v>7.874118682299393</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
✨ feat(analisis): Regenerar archivos Excel con datos verificados y agregar resultados detallados al informe para mejorar la claridad y robustez del análisis estadístico.
</commit_message>
<xml_diff>
--- a/analisis/02_PASO2_LEVENE_HOMOGENEIDAD_VARIANZAS.xlsx
+++ b/analisis/02_PASO2_LEVENE_HOMOGENEIDAD_VARIANZAS.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Levene" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Levene_N12" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -16,10 +16,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0000"/>
-  </numFmts>
-  <fonts count="3">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -30,23 +28,13 @@
     <font>
       <b val="1"/>
     </font>
-    <font>
-      <b val="1"/>
-      <color rgb="00FFFFFF"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="004472C4"/>
-        <bgColor rgb="004472C4"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -67,22 +55,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -449,209 +425,223 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="10" customWidth="1" min="1" max="1"/>
-    <col width="18" customWidth="1" min="2" max="2"/>
-    <col width="8" customWidth="1" min="3" max="3"/>
-    <col width="10" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="15" customWidth="1" min="6" max="6"/>
-    <col width="15" customWidth="1" min="7" max="7"/>
-    <col width="12" customWidth="1" min="8" max="8"/>
-    <col width="25" customWidth="1" min="9" max="9"/>
-  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
-        <is>
-          <t>nivel</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>metrica</t>
-        </is>
-      </c>
-      <c r="C1" s="2" t="inlineStr">
-        <is>
-          <t>n_ia</t>
-        </is>
-      </c>
-      <c r="D1" s="2" t="inlineStr">
-        <is>
-          <t>n_manual</t>
-        </is>
-      </c>
-      <c r="E1" s="2" t="inlineStr">
-        <is>
-          <t>var_ia</t>
-        </is>
-      </c>
-      <c r="F1" s="2" t="inlineStr">
-        <is>
-          <t>var_manual</t>
-        </is>
-      </c>
-      <c r="G1" s="2" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Nivel</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Metrica</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>N_Manual</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>N_IA</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Var_Manual</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Var_IA</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>F_statistic</t>
         </is>
       </c>
-      <c r="H1" s="2" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>p_value</t>
         </is>
       </c>
-      <c r="I1" s="2" t="inlineStr">
-        <is>
-          <t>es_igual</t>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Var_Iguales</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Test_Usar</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>N=12</t>
         </is>
       </c>
-      <c r="B2" s="3" t="inlineStr">
-        <is>
-          <t>instr_pct</t>
-        </is>
-      </c>
-      <c r="C2" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="D2" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="E2" s="5" t="n">
-        <v>128.958333</v>
-      </c>
-      <c r="F2" s="5" t="n">
-        <v>156.370833</v>
-      </c>
-      <c r="G2" s="5" t="n">
-        <v>0.1006</v>
-      </c>
-      <c r="H2" s="5" t="n">
-        <v>0.7577</v>
-      </c>
-      <c r="I2" s="3" t="inlineStr">
-        <is>
-          <t>✓ Varianzas IGUALES</t>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Instruction Coverage (%)</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>6</v>
+      </c>
+      <c r="D2" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2" t="n">
+        <v>156.3169366666667</v>
+      </c>
+      <c r="F2" t="n">
+        <v>129.098323375</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.1005534588048403</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.7576877767997356</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>t-Student</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="inlineStr">
+      <c r="A3" t="inlineStr">
         <is>
           <t>N=12</t>
         </is>
       </c>
-      <c r="B3" s="3" t="inlineStr">
-        <is>
-          <t>branch_pct</t>
-        </is>
-      </c>
-      <c r="C3" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="D3" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="E3" s="5" t="n">
-        <v>159.159722</v>
-      </c>
-      <c r="F3" s="5" t="n">
-        <v>159.159722</v>
-      </c>
-      <c r="G3" s="5" t="n">
-        <v>0.1262</v>
-      </c>
-      <c r="H3" s="5" t="n">
-        <v>0.7298</v>
-      </c>
-      <c r="I3" s="3" t="inlineStr">
-        <is>
-          <t>✓ Varianzas IGUALES</t>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Branch Coverage (%)</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>6</v>
+      </c>
+      <c r="D3" t="n">
+        <v>6</v>
+      </c>
+      <c r="E3" t="n">
+        <v>159.1666666666666</v>
+      </c>
+      <c r="F3" t="n">
+        <v>90.09130859375</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.1261631285169443</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.7298213975322283</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>t-Student</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="inlineStr">
+      <c r="A4" t="inlineStr">
         <is>
           <t>N=12</t>
         </is>
       </c>
-      <c r="B4" s="3" t="inlineStr">
-        <is>
-          <t>mutation_score</t>
-        </is>
-      </c>
-      <c r="C4" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="D4" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="E4" s="5" t="n">
-        <v>313.128333</v>
-      </c>
-      <c r="F4" s="5" t="n">
-        <v>313.756667</v>
-      </c>
-      <c r="G4" s="5" t="n">
-        <v>0.393</v>
-      </c>
-      <c r="H4" s="5" t="n">
-        <v>0.5448</v>
-      </c>
-      <c r="I4" s="3" t="inlineStr">
-        <is>
-          <t>✓ Varianzas IGUALES</t>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Mutation Score (%)</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>6</v>
+      </c>
+      <c r="D4" t="n">
+        <v>6</v>
+      </c>
+      <c r="E4" t="n">
+        <v>313.75844</v>
+      </c>
+      <c r="F4" t="n">
+        <v>134.87492959375</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.3930361867634057</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.5447541451208455</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>t-Student</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="inlineStr">
+      <c r="A5" t="inlineStr">
         <is>
           <t>N=12</t>
         </is>
       </c>
-      <c r="B5" s="3" t="inlineStr">
-        <is>
-          <t>time_seconds</t>
-        </is>
-      </c>
-      <c r="C5" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="D5" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="E5" s="5" t="n">
-        <v>0.007433</v>
-      </c>
-      <c r="F5" s="5" t="n">
-        <v>0.004736</v>
-      </c>
-      <c r="G5" s="5" t="n">
-        <v>6.3679</v>
-      </c>
-      <c r="H5" s="5" t="n">
-        <v>0.0302</v>
-      </c>
-      <c r="I5" s="3" t="inlineStr">
-        <is>
-          <t>✗ Varianzas DESIGUALES</t>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Time (seconds)</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>6</v>
+      </c>
+      <c r="D5" t="n">
+        <v>6</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.004736459427878402</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.03729544366901042</v>
+      </c>
+      <c r="G5" t="n">
+        <v>6.367874425075419</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.03020741164808924</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>t-Student Welch</t>
         </is>
       </c>
     </row>

</xml_diff>